<commit_message>
agregar v2 para casos de prueba
</commit_message>
<xml_diff>
--- a/data/DataDriven.xlsx
+++ b/data/DataDriven.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/cfloresh_emeal_nttdata_com/Documents/Escritorio/arquetipo_pruebas_E2E_automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{88615439-375A-4C2B-8A19-A297B79529E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EF687BB-A063-499E-BD16-C1790D4425A1}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{88615439-375A-4C2B-8A19-A297B79529E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDDEE0D0-AEB5-491E-878E-427D6BBEFE17}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{4CEB8AB6-E7B5-4B0E-B37E-4FFA86E7928B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{4CEB8AB6-E7B5-4B0E-B37E-4FFA86E7928B}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="2" r:id="rId1"/>
@@ -499,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC26A45-1F6A-4878-9929-72021F9E6239}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08E51A8-52B3-423D-BAD0-0E676C46E6EB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>